<commit_message>
make webpage to send meesage
</commit_message>
<xml_diff>
--- a/numbers_list/num.xlsx
+++ b/numbers_list/num.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Project\Whatsapp_auto_js\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Project\Whatsapp_auto_js\numbers_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E9CEB0-CC43-4E97-BB84-072F46C80E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA955F7-AA60-4930-86DD-F3E23C376A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F75396AA-D1B0-4A54-8CD0-507BF44C1165}"/>
   </bookViews>
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -376,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D921184C-5AAA-46A2-A8BC-DF99DDE2BCEB}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,7 +390,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>919098221369</v>
+        <v>917514074672</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -402,11 +398,6 @@
         <v>917514008774</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>919343865508</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>